<commit_message>
small changes to initial wrangling and document, and am ready for sql dumps
</commit_message>
<xml_diff>
--- a/docs/Project Workflow Documention/Data Pipeline Architecture/1.0-ss-Fishbit_Initial_Wrangling_Doc.xlsx
+++ b/docs/Project Workflow Documention/Data Pipeline Architecture/1.0-ss-Fishbit_Initial_Wrangling_Doc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="237">
   <si>
     <t>Original Column Names</t>
   </si>
@@ -184,12 +184,18 @@
     <t>originalStartTime</t>
   </si>
   <si>
+    <t>Not needed, duplicate values</t>
+  </si>
+  <si>
     <t>originalDuration</t>
   </si>
   <si>
     <t>elevationGain</t>
   </si>
   <si>
+    <t>Not needed, missing values</t>
+  </si>
+  <si>
     <t>hasActiveZoneMinutes</t>
   </si>
   <si>
@@ -232,135 +238,126 @@
     <t>intervalWorkoutData.intervalSummaries</t>
   </si>
   <si>
+    <t>intervalWorkoutData.numRepeats</t>
+  </si>
+  <si>
+    <t>activeZoneMinutes.totalMinutes</t>
+  </si>
+  <si>
+    <t>Duplicate Data</t>
+  </si>
+  <si>
+    <t>activeZoneMinutes.minutesInHeartRateZones</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>pace</t>
+  </si>
+  <si>
+    <t>distanceUnit</t>
+  </si>
+  <si>
+    <t>hrz_OutofRange_calories</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>Expansion of heartRateZones column</t>
+  </si>
+  <si>
+    <t>hrz_FatBurn_calories</t>
+  </si>
+  <si>
+    <t>hrz_Cardio_calories</t>
+  </si>
+  <si>
+    <t>hrz_Peak_calories</t>
+  </si>
+  <si>
+    <t>hrz_OutofRange_minutes</t>
+  </si>
+  <si>
+    <t>int32</t>
+  </si>
+  <si>
+    <t>hrz_FatBurn_minutes</t>
+  </si>
+  <si>
+    <t>hrz_Cardio_minutes</t>
+  </si>
+  <si>
+    <t>hrz_Peak_minutes</t>
+  </si>
+  <si>
+    <t>dateOfSleep</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>endTime</t>
+  </si>
+  <si>
+    <t>infoCode</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>isMainSleep</t>
+  </si>
+  <si>
+    <t>Not needed, internal API usage</t>
+  </si>
+  <si>
+    <t>minutesAfterWakeup</t>
+  </si>
+  <si>
+    <t>No metadata found on this column</t>
+  </si>
+  <si>
+    <t>minutesAsleep</t>
+  </si>
+  <si>
+    <t>minutesAwake</t>
+  </si>
+  <si>
+    <t>minutesToFallAsleep</t>
+  </si>
+  <si>
+    <t>All 0</t>
+  </si>
+  <si>
+    <t>timeInBed</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>levels.data</t>
+  </si>
+  <si>
+    <t>Expanded in another table</t>
+  </si>
+  <si>
+    <t>levels.shortData</t>
+  </si>
+  <si>
+    <t>levels.summary.deep.count</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>shorter name</t>
-  </si>
-  <si>
-    <t>intervalWorkoutData.numRepeats</t>
-  </si>
-  <si>
-    <t>iwd_numRepeats</t>
-  </si>
-  <si>
-    <t>activeZoneMinutes.totalMinutes</t>
-  </si>
-  <si>
-    <t>Duplicate Data</t>
-  </si>
-  <si>
-    <t>activeZoneMinutes.minutesInHeartRateZones</t>
-  </si>
-  <si>
-    <t>distance</t>
-  </si>
-  <si>
-    <t>speed</t>
-  </si>
-  <si>
-    <t>pace</t>
-  </si>
-  <si>
-    <t>distanceUnit</t>
-  </si>
-  <si>
-    <t>hrz_OutofRange_calories</t>
-  </si>
-  <si>
-    <t>Added</t>
-  </si>
-  <si>
-    <t>Expansion of heartRateZones column</t>
-  </si>
-  <si>
-    <t>hrz_FatBurn_calories</t>
-  </si>
-  <si>
-    <t>hrz_Cardio_calories</t>
-  </si>
-  <si>
-    <t>hrz_Peak_calories</t>
-  </si>
-  <si>
-    <t>hrz_OutofRange_minutes</t>
-  </si>
-  <si>
-    <t>int32</t>
-  </si>
-  <si>
-    <t>hrz_FatBurn_minutes</t>
-  </si>
-  <si>
-    <t>hrz_Cardio_minutes</t>
-  </si>
-  <si>
-    <t>hrz_Peak_minutes</t>
-  </si>
-  <si>
-    <t>dateOfSleep</t>
-  </si>
-  <si>
-    <t>efficiency</t>
-  </si>
-  <si>
-    <t>endTime</t>
-  </si>
-  <si>
-    <t>infoCode</t>
-  </si>
-  <si>
-    <t>Removed</t>
-  </si>
-  <si>
-    <t>isMainSleep</t>
-  </si>
-  <si>
-    <t>Not needed, internal API usage</t>
-  </si>
-  <si>
-    <t>minutesAfterWakeup</t>
-  </si>
-  <si>
-    <t>No metadata found on this column</t>
-  </si>
-  <si>
-    <t>minutesAsleep</t>
-  </si>
-  <si>
-    <t>minutesAwake</t>
-  </si>
-  <si>
-    <t>minutesToFallAsleep</t>
-  </si>
-  <si>
-    <t>All 0</t>
-  </si>
-  <si>
-    <t>timeInBed</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>levels.data</t>
-  </si>
-  <si>
     <t>Shorter</t>
   </si>
   <si>
-    <t>sc_data</t>
-  </si>
-  <si>
-    <t>levels.shortData</t>
-  </si>
-  <si>
-    <t>sc_shortData</t>
-  </si>
-  <si>
-    <t>levels.summary.deep.count</t>
-  </si>
-  <si>
     <t>sc_deep_count</t>
   </si>
   <si>
@@ -466,7 +463,46 @@
     <t>sc_restless_minutes</t>
   </si>
   <si>
+    <t>Created an additional table</t>
+  </si>
+  <si>
+    <t>Column Names</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>sleep_id</t>
+  </si>
+  <si>
+    <t>id of sleep row belongs to</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>indicating whether it is a shortData value or not (see table above)</t>
+  </si>
+  <si>
     <t>dateTime</t>
+  </si>
+  <si>
+    <t>string of datetime</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>level of sleep (deep, rem, etc...)</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>length of level at that certain time</t>
   </si>
   <si>
     <t>value.nightlyRelative</t>
@@ -937,7 +973,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1049,6 +1085,33 @@
     <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1061,15 +1124,13 @@
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1113,7 +1174,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="7">
+  <tableStyles count="8">
     <tableStyle count="3" pivot="0" name="Sheet1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1145,6 +1206,11 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Sheet1-style 7">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Sheet1-style 8">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1208,21 +1274,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A89:F91" displayName="Skin" name="Skin" id="3">
-  <tableColumns count="6">
-    <tableColumn name="Original Column Names" id="1"/>
-    <tableColumn name="OriginalType" id="2"/>
-    <tableColumn name="Change" id="3"/>
-    <tableColumn name="Reason" id="4"/>
-    <tableColumn name="Final Column Names" id="5"/>
-    <tableColumn name="Final Type" id="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A91:E96" displayName="initial_clean_sleep_levels" name="initial_clean_sleep_levels" id="3">
+  <tableColumns count="5">
+    <tableColumn name="Column Names" id="1"/>
+    <tableColumn name="Type" id="2"/>
+    <tableColumn name="Function" id="3"/>
+    <tableColumn name="Column 1" id="4"/>
+    <tableColumn name="Column 5" id="5"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A93:F96" displayName="HRV" name="HRV" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A102:F104" displayName="Skin" name="Skin" id="4">
   <tableColumns count="6">
     <tableColumn name="Original Column Names" id="1"/>
     <tableColumn name="OriginalType" id="2"/>
@@ -1236,7 +1301,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A98:F100" displayName="BRV" name="BRV" id="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A106:F109" displayName="HRV" name="HRV" id="5">
   <tableColumns count="6">
     <tableColumn name="Original Column Names" id="1"/>
     <tableColumn name="OriginalType" id="2"/>
@@ -1250,7 +1315,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A104:F124" displayName="MFP" name="MFP" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A111:F113" displayName="BRV" name="BRV" id="6">
   <tableColumns count="6">
     <tableColumn name="Original Column Names" id="1"/>
     <tableColumn name="OriginalType" id="2"/>
@@ -1264,7 +1329,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A126:F139" displayName="Google_Form" name="Google_Form" id="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A117:F137" displayName="MFP" name="MFP" id="7">
   <tableColumns count="6">
     <tableColumn name="Original Column Names" id="1"/>
     <tableColumn name="OriginalType" id="2"/>
@@ -1274,6 +1339,20 @@
     <tableColumn name="Final Type" id="6"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 7" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A139:F152" displayName="Google_Form" name="Google_Form" id="8">
+  <tableColumns count="6">
+    <tableColumn name="Original Column Names" id="1"/>
+    <tableColumn name="OriginalType" id="2"/>
+    <tableColumn name="Change" id="3"/>
+    <tableColumn name="Reason" id="4"/>
+    <tableColumn name="Final Column Names" id="5"/>
+    <tableColumn name="Final Type" id="6"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet1-style 8" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1477,10 +1556,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -2253,7 +2329,7 @@
         <v>30</v>
       </c>
       <c r="G19" s="11" t="str">
-        <f t="shared" ref="G19:G23" si="6">"'" &amp; E19  &amp; "'" &amp; " : '" &amp; F19 &amp; "'"</f>
+        <f>"'" &amp; E19  &amp; "'" &amp; " : '" &amp; F19 &amp; "'"</f>
         <v>'startTime' : 'Object'</v>
       </c>
       <c r="H19" s="13"/>
@@ -2281,19 +2357,14 @@
         <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>'originalStartTime' : 'Object'</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -2313,25 +2384,20 @@
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v>'originalDuration' : 'int64'</v>
-      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -2351,25 +2417,20 @@
     </row>
     <row r="22">
       <c r="A22" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>'elevationGain' : 'float64'</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -2389,7 +2450,7 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>48</v>
@@ -2399,13 +2460,13 @@
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G23" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f>"'" &amp; E23  &amp; "'" &amp; " : '" &amp; F23 &amp; "'"</f>
         <v>'hasActiveZoneMinutes' : 'bool'</v>
       </c>
       <c r="H23" s="13"/>
@@ -2427,7 +2488,7 @@
     </row>
     <row r="24">
       <c r="A24" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>48</v>
@@ -2441,7 +2502,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H24" s="17" t="str">
         <f>A25</f>
@@ -2468,7 +2529,7 @@
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>30</v>
@@ -2477,7 +2538,7 @@
         <v>25</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
@@ -2501,7 +2562,7 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>30</v>
@@ -2510,7 +2571,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -2534,7 +2595,7 @@
     </row>
     <row r="27">
       <c r="A27" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>30</v>
@@ -2543,7 +2604,7 @@
         <v>25</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -2567,7 +2628,7 @@
     </row>
     <row r="28">
       <c r="A28" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>30</v>
@@ -2576,7 +2637,7 @@
         <v>25</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -2600,7 +2661,7 @@
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>30</v>
@@ -2609,7 +2670,7 @@
         <v>25</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -2633,7 +2694,7 @@
     </row>
     <row r="30">
       <c r="A30" s="15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>48</v>
@@ -2648,12 +2709,12 @@
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="str">
-        <f t="shared" ref="H30:H32" si="7">A31</f>
+        <f t="shared" ref="H30:H32" si="6">A31</f>
         <v>manualValuesSpecified.distance</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7" t="str">
-        <f t="shared" ref="J30:J32" si="8">"'" &amp; G30 &amp; "'"</f>
+        <f t="shared" ref="J30:J32" si="7">"'" &amp; G30 &amp; "'"</f>
         <v>''</v>
       </c>
       <c r="K30" s="7"/>
@@ -2672,7 +2733,7 @@
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>48</v>
@@ -2687,12 +2748,12 @@
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
       <c r="H31" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>manualValuesSpecified.steps</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>''</v>
       </c>
       <c r="K31" s="19"/>
@@ -2711,7 +2772,7 @@
     </row>
     <row r="32">
       <c r="A32" s="15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>48</v>
@@ -2725,15 +2786,15 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H32" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>intervalWorkoutData.intervalSummaries</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>'iwd_intervalSummaries'</v>
       </c>
       <c r="K32" s="7"/>
@@ -2752,27 +2813,20 @@
     </row>
     <row r="33">
       <c r="A33" s="21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G33" s="11" t="str">
-        <f t="shared" ref="G33:G34" si="9">"'" &amp; E33  &amp; "'" &amp; " : '" &amp; F33 &amp; "'"</f>
-        <v>'iwd_intervalSummaries' : 'Object'</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
@@ -2798,21 +2852,14 @@
         <v>24</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>'iwd_numRepeats' : 'int64'</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
@@ -2832,7 +2879,7 @@
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>24</v>
@@ -2841,18 +2888,18 @@
         <v>25</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="19" t="str">
-        <f t="shared" ref="H35:H40" si="10">A36</f>
+        <f t="shared" ref="H35:H40" si="8">A36</f>
         <v>activeZoneMinutes.minutesInHeartRateZones</v>
       </c>
       <c r="I35" s="19"/>
       <c r="J35" s="19" t="str">
-        <f t="shared" ref="J35:J40" si="11">"'" &amp; G35 &amp; "'"</f>
+        <f t="shared" ref="J35:J40" si="9">"'" &amp; G35 &amp; "'"</f>
         <v>''</v>
       </c>
       <c r="K35" s="19"/>
@@ -2871,7 +2918,7 @@
     </row>
     <row r="36">
       <c r="A36" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>30</v>
@@ -2880,18 +2927,18 @@
         <v>25</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>distance</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>''</v>
       </c>
       <c r="K36" s="7"/>
@@ -2910,7 +2957,7 @@
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>33</v>
@@ -2925,12 +2972,12 @@
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
       <c r="H37" s="19" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>speed</v>
       </c>
       <c r="I37" s="19"/>
       <c r="J37" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>''</v>
       </c>
       <c r="K37" s="19"/>
@@ -2949,7 +2996,7 @@
     </row>
     <row r="38">
       <c r="A38" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>33</v>
@@ -2964,12 +3011,12 @@
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>pace</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>''</v>
       </c>
       <c r="K38" s="7"/>
@@ -2988,7 +3035,7 @@
     </row>
     <row r="39">
       <c r="A39" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>33</v>
@@ -3003,12 +3050,12 @@
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>distanceUnit</v>
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>''</v>
       </c>
       <c r="K39" s="19"/>
@@ -3027,7 +3074,7 @@
     </row>
     <row r="40">
       <c r="A40" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>30</v>
@@ -3041,15 +3088,15 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H40" s="7" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="7" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>'hrz_OutofRange_calories'</v>
       </c>
       <c r="K40" s="7"/>
@@ -3070,19 +3117,19 @@
       <c r="A41" s="22"/>
       <c r="B41" s="19"/>
       <c r="C41" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="E41" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G41" s="11" t="str">
-        <f t="shared" ref="G41:G48" si="12">"'" &amp; E41  &amp; "'" &amp; " : '" &amp; F41 &amp; "'"</f>
+        <f t="shared" ref="G41:G48" si="10">"'" &amp; E41  &amp; "'" &amp; " : '" &amp; F41 &amp; "'"</f>
         <v>'hrz_OutofRange_calories' : 'float64'</v>
       </c>
       <c r="H41" s="13"/>
@@ -3106,19 +3153,19 @@
       <c r="A42" s="23"/>
       <c r="B42" s="7"/>
       <c r="C42" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="16" t="s">
-        <v>86</v>
-      </c>
       <c r="F42" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G42" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>'hrz_FatBurn_calories' : 'float64'</v>
       </c>
       <c r="H42" s="17"/>
@@ -3142,19 +3189,19 @@
       <c r="A43" s="22"/>
       <c r="B43" s="19"/>
       <c r="C43" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="E43" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F43" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G43" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>'hrz_Cardio_calories' : 'float64'</v>
       </c>
       <c r="H43" s="13"/>
@@ -3178,19 +3225,19 @@
       <c r="A44" s="23"/>
       <c r="B44" s="7"/>
       <c r="C44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="E44" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G44" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>'hrz_Peak_calories' : 'float64'</v>
       </c>
       <c r="H44" s="17"/>
@@ -3214,19 +3261,19 @@
       <c r="A45" s="22"/>
       <c r="B45" s="19"/>
       <c r="C45" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="E45" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F45" s="11" t="s">
-        <v>90</v>
-      </c>
       <c r="G45" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>'hrz_OutofRange_minutes' : 'int32'</v>
       </c>
       <c r="H45" s="13"/>
@@ -3250,19 +3297,19 @@
       <c r="A46" s="23"/>
       <c r="B46" s="7"/>
       <c r="C46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="E46" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G46" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>'hrz_FatBurn_minutes' : 'int32'</v>
       </c>
       <c r="H46" s="17"/>
@@ -3286,19 +3333,19 @@
       <c r="A47" s="22"/>
       <c r="B47" s="19"/>
       <c r="C47" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="E47" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G47" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>'hrz_Cardio_minutes' : 'int32'</v>
       </c>
       <c r="H47" s="13"/>
@@ -3322,19 +3369,19 @@
       <c r="A48" s="24"/>
       <c r="B48" s="25"/>
       <c r="C48" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="26" t="s">
-        <v>85</v>
-      </c>
       <c r="E48" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F48" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G48" s="26" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>'hrz_Peak_minutes' : 'int32'</v>
       </c>
       <c r="H48" s="28" t="str">
@@ -3382,7 +3429,7 @@
     </row>
     <row r="53">
       <c r="A53" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>30</v>
@@ -3390,7 +3437,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F53" s="32" t="s">
         <v>30</v>
@@ -3444,7 +3491,7 @@
     </row>
     <row r="55">
       <c r="A55" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>24</v>
@@ -3452,15 +3499,15 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F55" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>30</v>
@@ -3468,7 +3515,7 @@
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F56" s="33" t="s">
         <v>30</v>
@@ -3476,13 +3523,13 @@
     </row>
     <row r="57">
       <c r="A57" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>49</v>
@@ -3492,7 +3539,7 @@
     </row>
     <row r="58">
       <c r="A58" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>48</v>
@@ -3500,7 +3547,7 @@
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
       <c r="E58" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F58" s="33" t="s">
         <v>48</v>
@@ -3514,10 +3561,10 @@
         <v>24</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="32"/>
@@ -3530,7 +3577,7 @@
         <v>30</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>40</v>
@@ -3540,23 +3587,23 @@
     </row>
     <row r="61">
       <c r="A61" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="32"/>
     </row>
     <row r="62">
       <c r="A62" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>24</v>
@@ -3564,7 +3611,7 @@
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
       <c r="E62" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F62" s="33" t="s">
         <v>24</v>
@@ -3572,7 +3619,7 @@
     </row>
     <row r="63">
       <c r="A63" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>24</v>
@@ -3580,7 +3627,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F63" s="32" t="s">
         <v>24</v>
@@ -3588,16 +3635,16 @@
     </row>
     <row r="64">
       <c r="A64" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E64" s="11"/>
       <c r="F64" s="33"/>
@@ -3620,7 +3667,7 @@
     </row>
     <row r="66">
       <c r="A66" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>24</v>
@@ -3628,7 +3675,7 @@
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
       <c r="E66" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F66" s="33" t="s">
         <v>24</v>
@@ -3636,7 +3683,7 @@
     </row>
     <row r="67">
       <c r="A67" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>30</v>
@@ -3644,7 +3691,7 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F67" s="32" t="s">
         <v>30</v>
@@ -3652,59 +3699,51 @@
     </row>
     <row r="68">
       <c r="A68" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="F68" s="33" t="s">
-        <v>30</v>
-      </c>
+      <c r="E68" s="11"/>
+      <c r="F68" s="33"/>
     </row>
     <row r="69">
       <c r="A69" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E69" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>30</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="32"/>
     </row>
     <row r="70">
       <c r="A70" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>115</v>
       </c>
       <c r="F70" s="33" t="s">
         <v>33</v>
@@ -3712,19 +3751,19 @@
     </row>
     <row r="71">
       <c r="A71" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E71" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="F71" s="32" t="s">
         <v>33</v>
@@ -3732,19 +3771,19 @@
     </row>
     <row r="72">
       <c r="A72" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E72" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="F72" s="33" t="s">
         <v>33</v>
@@ -3752,19 +3791,19 @@
     </row>
     <row r="73">
       <c r="A73" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="F73" s="32" t="s">
         <v>33</v>
@@ -3772,19 +3811,19 @@
     </row>
     <row r="74">
       <c r="A74" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E74" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="F74" s="33" t="s">
         <v>33</v>
@@ -3792,19 +3831,19 @@
     </row>
     <row r="75">
       <c r="A75" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E75" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="F75" s="32" t="s">
         <v>33</v>
@@ -3812,19 +3851,19 @@
     </row>
     <row r="76">
       <c r="A76" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="F76" s="33" t="s">
         <v>33</v>
@@ -3832,19 +3871,19 @@
     </row>
     <row r="77">
       <c r="A77" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E77" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>129</v>
       </c>
       <c r="F77" s="32" t="s">
         <v>33</v>
@@ -3852,19 +3891,19 @@
     </row>
     <row r="78">
       <c r="A78" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E78" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>131</v>
       </c>
       <c r="F78" s="33" t="s">
         <v>33</v>
@@ -3872,19 +3911,19 @@
     </row>
     <row r="79">
       <c r="A79" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E79" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>133</v>
       </c>
       <c r="F79" s="32" t="s">
         <v>33</v>
@@ -3892,19 +3931,19 @@
     </row>
     <row r="80">
       <c r="A80" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E80" s="12" t="s">
         <v>134</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="F80" s="33" t="s">
         <v>33</v>
@@ -3912,19 +3951,19 @@
     </row>
     <row r="81">
       <c r="A81" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E81" s="16" t="s">
         <v>136</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E81" s="16" t="s">
-        <v>137</v>
       </c>
       <c r="F81" s="32" t="s">
         <v>33</v>
@@ -3932,19 +3971,19 @@
     </row>
     <row r="82">
       <c r="A82" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E82" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F82" s="33" t="s">
         <v>33</v>
@@ -3952,19 +3991,19 @@
     </row>
     <row r="83">
       <c r="A83" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E83" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="F83" s="32" t="s">
         <v>33</v>
@@ -3972,19 +4011,19 @@
     </row>
     <row r="84">
       <c r="A84" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E84" s="12" t="s">
         <v>142</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="F84" s="33" t="s">
         <v>33</v>
@@ -3992,19 +4031,19 @@
     </row>
     <row r="85">
       <c r="A85" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E85" s="16" t="s">
         <v>144</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E85" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="F85" s="32" t="s">
         <v>33</v>
@@ -4012,19 +4051,19 @@
     </row>
     <row r="86">
       <c r="A86" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E86" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>147</v>
       </c>
       <c r="F86" s="33" t="s">
         <v>33</v>
@@ -4032,1087 +4071,1193 @@
     </row>
     <row r="87">
       <c r="A87" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="E87" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="B87" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C87" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D87" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="E87" s="27" t="s">
+      <c r="F87" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="F87" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="s">
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D91" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D92" s="41"/>
+      <c r="E92" s="42"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D93" s="19"/>
+      <c r="E93" s="20"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D94" s="7"/>
+      <c r="E94" s="8"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D95" s="19"/>
+      <c r="E95" s="20"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="B96" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="D96" s="25"/>
+      <c r="E96" s="45"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E102" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F89" s="3" t="s">
+      <c r="F102" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C90" s="5" t="s">
+    <row r="103">
+      <c r="A103" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C103" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="B91" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C91" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D91" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E91" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="F91" s="39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="s">
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="B104" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="D104" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="E104" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="F104" s="48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="E106" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="F106" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D94" s="7"/>
-      <c r="E94" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F94" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="B95" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="E95" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="F95" s="33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="B96" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C96" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D96" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E96" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="F96" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D99" s="7"/>
-      <c r="E99" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F99" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="B100" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C100" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D100" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E100" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="F100" s="39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F105" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G105" s="41" t="str">
-        <f t="shared" ref="G105:G139" si="13"> "'" &amp; A105 &amp; "'" &amp; " : '" &amp; E105 &amp; "'"</f>
-        <v>'Date' : 'date'</v>
-      </c>
-      <c r="H105" s="41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="B106" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C106" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D106" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F106" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G106" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Meal' : 'meal'</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>161</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D107" s="7"/>
       <c r="E107" s="5" t="s">
-        <v>31</v>
+        <v>157</v>
       </c>
       <c r="F107" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G107" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Calories' : 'calories'</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E108" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B108" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D108" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E108" s="11" t="s">
+      <c r="F108" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="F108" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G108" s="41" t="str">
-        <f t="shared" si="13"/>
+      <c r="B109" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D109" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F109" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112" s="7"/>
+      <c r="E112" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F112" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="B113" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C113" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="D113" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="E113" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="F113" s="48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F118" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H118" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F119" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G119" s="37" t="str">
+        <f t="shared" ref="G119:G153" si="11"> "'" &amp; A118 &amp; "'" &amp; " : '" &amp; E118 &amp; "'"</f>
+        <v>'Date' : 'date'</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F120" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G120" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Meal' : 'meal'</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F121" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G121" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Calories' : 'calories'</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F122" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G122" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'Fat (g)' : 'fat_g'</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F109" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G109" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="123">
+      <c r="A123" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="F123" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G123" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'Saturated Fat' : 'sat_fat'</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E110" s="11" t="s">
+    <row r="124">
+      <c r="A124" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F124" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G124" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Polyunsaturated Fat' : 'poly_fat'</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E125" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F125" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G125" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Monounsaturated Fat' : 'mono_fat'</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F126" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G126" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Trans Fat' : 'trans_fat'</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D127" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F127" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G127" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Cholesterol' : 'cholesterol'</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F128" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G128" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Sodium (mg)' : 'sodium_mg'</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C129" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E129" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F129" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G129" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Potassium' : 'potassium'</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F130" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G130" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Carbohydrates (g)' : 'carbohydrates_g'</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="B131" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C131" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D131" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E131" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F131" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G131" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Fiber' : 'fiber_g'</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F132" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G132" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Sugar' : 'sugar'</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C133" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E133" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F133" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G133" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Protein (g)' : 'protein_g'</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F134" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G134" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Vitamin A' : 'vitamin_a'</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C135" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D135" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E135" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F135" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G135" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Vitamin C' : 'vitamin_c'</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F136" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G136" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Calcium' : 'calcium'</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="B137" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C137" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D137" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="E137" s="50"/>
+      <c r="F137" s="51"/>
+      <c r="G137" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Iron' : 'iron'</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="G138" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Note' : ''</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G139" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'' : ''</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F140" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G140" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'Original Column Names' : 'Final Column Names'</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="F110" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G110" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Polyunsaturated Fat' : 'poly_fat'</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E111" s="5" t="s">
+      <c r="B141" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C141" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D141" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E141" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="F111" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G111" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Monounsaturated Fat' : 'mono_fat'</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C112" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D112" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E112" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="F112" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G112" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Trans Fat' : 'trans_fat'</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E113" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F113" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G113" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Cholesterol' : 'cholesterol'</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="B114" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C114" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D114" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E114" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="F114" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G114" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Sodium (mg)' : 'sodium_mg'</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E115" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="F115" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G115" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Potassium' : 'potassium'</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D116" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E116" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="F116" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G116" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Carbohydrates (g)' : 'carbohydrates_g'</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E117" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F117" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G117" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Fiber' : 'fiber_g'</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="B118" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C118" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D118" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E118" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="F118" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G118" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Sugar' : 'sugar'</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E119" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="F119" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G119" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Protein (g)' : 'protein_g'</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B120" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C120" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D120" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F120" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G120" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Vitamin A' : 'vitamin_a'</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="F121" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G121" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Vitamin C' : 'vitamin_c'</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="B122" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C122" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D122" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E122" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F122" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G122" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Calcium' : 'calcium'</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E123" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="F123" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G123" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Iron' : 'iron'</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="B124" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C124" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D124" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="E124" s="42"/>
-      <c r="F124" s="43"/>
-      <c r="G124" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Note' : ''</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="G125" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'' : ''</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F126" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G126" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v>'Original Column Names' : 'Final Column Names'</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D127" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E127" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F127" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G127" s="41" t="str">
-        <f t="shared" si="13"/>
+      <c r="F141" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G141" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'Timestamp' : 'timestamp'</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B128" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C128" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D128" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="E128" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="F128" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G128" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="142">
+      <c r="A142" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F142" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G142" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'Date' : 'date'</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C129" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D129" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E129" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="F129" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G129" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="143">
+      <c r="A143" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C143" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D143" s="19"/>
+      <c r="E143" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="F143" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G143" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'How do you feel about last night's sleep?' : 'last_sleep_feel'</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D130" s="19"/>
-      <c r="E130" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="F130" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="G130" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="144">
+      <c r="A144" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D144" s="7"/>
+      <c r="E144" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F144" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G144" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'What was last nights sleep score? (if form date is 8/7, then sleep score is sleep from 8/6-8/7)' : 'last_sleep_score'</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D131" s="7"/>
-      <c r="E131" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F131" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G131" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="145">
+      <c r="A145" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B145" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D145" s="19"/>
+      <c r="E145" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="F145" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G145" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'Any particular qualities?' : 'daily_particular_qualities'</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="B132" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C132" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D132" s="19"/>
-      <c r="E132" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="F132" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G132" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="146">
+      <c r="A146" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D146" s="7"/>
+      <c r="E146" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F146" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G146" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'How do you feel about the day?' : 'day_feel'</v>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D133" s="7"/>
-      <c r="E133" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="F133" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G133" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="147">
+      <c r="A147" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B147" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C147" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D147" s="19"/>
+      <c r="E147" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F147" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G147" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'Was there an external factor that impacted your day?' : 'ef_status'</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="B134" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C134" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D134" s="19"/>
-      <c r="E134" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="F134" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G134" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="148">
+      <c r="A148" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D148" s="7"/>
+      <c r="E148" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F148" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G148" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'What factor impacted your day?' : 'ef_description'</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D135" s="7"/>
-      <c r="E135" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="F135" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G135" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="149">
+      <c r="A149" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C149" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D149" s="19"/>
+      <c r="E149" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F149" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G149" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'Is there something you are dissatisfied with today?' : 'dissatisfied_status'</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="B136" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C136" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D136" s="19"/>
-      <c r="E136" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="F136" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="G136" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="150">
+      <c r="A150" s="23"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F150" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="G150" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'What was todays stress mgmnt score? (if I slept 9/10 -&gt; 9/11, look at 9/11 score)
 Insert as: score, responsiveness, exertion_balance, sleep_patterns' : 'stress_mgmt_score'</v>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" s="23"/>
-      <c r="B137" s="7"/>
-      <c r="C137" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D137" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E137" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="F137" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="G137" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="151">
+      <c r="A151" s="22"/>
+      <c r="B151" s="19"/>
+      <c r="C151" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D151" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E151" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F151" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G151" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'' : 'stress_responsiveness'</v>
       </c>
     </row>
-    <row r="138">
-      <c r="A138" s="22"/>
-      <c r="B138" s="19"/>
-      <c r="C138" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D138" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="E138" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="F138" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="G138" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="152">
+      <c r="A152" s="24"/>
+      <c r="B152" s="25"/>
+      <c r="C152" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D152" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="E152" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="F152" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G152" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'' : 'stress_exertion'</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" s="24"/>
-      <c r="B139" s="25"/>
-      <c r="C139" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D139" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="E139" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="F139" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="G139" s="41" t="str">
-        <f t="shared" si="13"/>
+    <row r="153">
+      <c r="G153" s="37" t="str">
+        <f t="shared" si="11"/>
         <v>'' : 'stress_sleep'</v>
       </c>
     </row>
+    <row r="157">
+      <c r="A157" s="52"/>
+      <c r="B157" s="52"/>
+      <c r="C157" s="52"/>
+      <c r="D157" s="52"/>
+      <c r="E157" s="52"/>
+      <c r="F157" s="52"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="52"/>
+      <c r="B158" s="52"/>
+      <c r="C158" s="52"/>
+      <c r="D158" s="52"/>
+      <c r="E158" s="52"/>
+      <c r="F158" s="52"/>
+    </row>
     <row r="211">
-      <c r="A211" s="41" t="s">
-        <v>163</v>
+      <c r="A211" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="41" t="s">
-        <v>163</v>
+      <c r="A218" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="41" t="s">
-        <v>163</v>
+      <c r="A219" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="41" t="s">
-        <v>163</v>
+      <c r="A220" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="41" t="s">
-        <v>163</v>
+      <c r="A225" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="41" t="s">
-        <v>163</v>
+      <c r="A226" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="41" t="s">
-        <v>163</v>
+      <c r="A227" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="41" t="s">
-        <v>163</v>
+      <c r="A228" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="41" t="s">
-        <v>163</v>
+      <c r="A229" s="37" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
-  <tableParts count="7">
-    <tablePart r:id="rId9"/>
+  <tableParts count="8">
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>